<commit_message>
no me peguen por pushear a main
</commit_message>
<xml_diff>
--- a/metricas de modelos.xlsx
+++ b/metricas de modelos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://finguy-my.sharepoint.com/personal/federico_gil_fing_edu_uy/Documents/Escritorio/Facultad/Semestre 11/ProyGrad/ProyGrad2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="204" documentId="11_F25DC773A252ABDACC1048AE815C7CCA5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54590293-4ECF-42CB-A17A-F6F9B067EEF0}"/>
+  <xr:revisionPtr revIDLastSave="288" documentId="11_F25DC773A252ABDACC1048AE815C7CCA5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2449D428-0153-444B-A6E1-ECC57AC07096}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Modelo</t>
   </si>
@@ -112,6 +112,9 @@
   <si>
     <t>Total AVG</t>
   </si>
+  <si>
+    <t>gpt-4o</t>
+  </si>
 </sst>
 </file>
 
@@ -168,10 +171,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -298,34 +301,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>gpt-4o</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>gpt-4-turbo-2024-04-09</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>mixtral8x7b</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>claude-instant-v1</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>llama3-70b-8192</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>claude-2.1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>gemma-8b-it</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>llama2-70b-chat</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>claude-2</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>gpt-3.5-turbo-0125</c:v>
                 </c:pt>
               </c:strCache>
@@ -333,35 +339,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$11</c:f>
+              <c:f>Sheet1!$C$3:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>0.42199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.42253521126760502</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.49295774647887303</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.47887323943661902</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.50704225352112597</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.40845070422535201</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.53521126760563298</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.52112676056338003</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.43661971830985902</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.54929577464788704</c:v>
                 </c:pt>
               </c:numCache>
@@ -399,34 +408,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>gpt-4o</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>gpt-4-turbo-2024-04-09</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>mixtral8x7b</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>claude-instant-v1</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>llama3-70b-8192</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>claude-2.1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>gemma-8b-it</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>llama2-70b-chat</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>claude-2</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>gpt-3.5-turbo-0125</c:v>
                 </c:pt>
               </c:strCache>
@@ -434,35 +446,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$11</c:f>
+              <c:f>Sheet1!$D$3:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>0.3548</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.25806451612903197</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.38709677419354799</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.41935483870967699</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.16129032258064499</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.29032258064516098</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.54838709677419295</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.19354838709677399</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.225806451612903</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.225806451612903</c:v>
                 </c:pt>
               </c:numCache>
@@ -500,34 +515,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>gpt-4o</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>gpt-4-turbo-2024-04-09</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>mixtral8x7b</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>claude-instant-v1</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>llama3-70b-8192</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>claude-2.1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>gemma-8b-it</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>llama2-70b-chat</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>claude-2</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>gpt-3.5-turbo-0125</c:v>
                 </c:pt>
               </c:strCache>
@@ -535,35 +553,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$11</c:f>
+              <c:f>Sheet1!$E$3:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>0.34920000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.28070175438596401</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.41269841269841201</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.22222222222222199</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.50746268656716398</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.26086956521739102</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.25925925925925902</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.30434782608695599</c:v>
                 </c:pt>
               </c:numCache>
@@ -880,34 +901,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>gpt-4o</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>gpt-4-turbo-2024-04-09</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>mixtral8x7b</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>claude-instant-v1</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>llama3-70b-8192</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>claude-2.1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>gemma-8b-it</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>llama2-70b-chat</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>claude-2</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>gpt-3.5-turbo-0125</c:v>
                 </c:pt>
               </c:strCache>
@@ -915,35 +939,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$11</c:f>
+              <c:f>Sheet1!$F$3:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>0.94110000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.91420000000000001</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.70579999999999998</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.68569999999999998</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.81420000000000003</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.72719999999999996</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.48570000000000002</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.61529999999999996</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.7</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.62309999999999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -981,34 +1008,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>gpt-4o</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>gpt-4-turbo-2024-04-09</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>mixtral8x7b</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>claude-instant-v1</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>llama3-70b-8192</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>claude-2.1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>gemma-8b-it</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>llama2-70b-chat</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>claude-2</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>gpt-3.5-turbo-0125</c:v>
                 </c:pt>
               </c:strCache>
@@ -1016,35 +1046,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$11</c:f>
+              <c:f>Sheet1!$G$3:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>0.94099999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.91610000000000003</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.70879999999999999</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.7006</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.81410000000000005</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.73609999999999998</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.49909999999999999</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.73609999999999998</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.70140000000000002</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.49909999999999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -1082,34 +1115,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>gpt-4o</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>gpt-4-turbo-2024-04-09</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>mixtral8x7b</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>claude-instant-v1</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>llama3-70b-8192</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>claude-2.1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>gemma-8b-it</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>llama2-70b-chat</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>claude-2</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>gpt-3.5-turbo-0125</c:v>
                 </c:pt>
               </c:strCache>
@@ -1117,35 +1153,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$3:$H$11</c:f>
+              <c:f>Sheet1!$H$3:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>0.94110000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.91320000000000001</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.7026</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.68069999999999997</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.81100000000000005</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.72829999999999995</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.4834</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.72829999999999995</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.70220000000000005</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.4834</c:v>
                 </c:pt>
               </c:numCache>
@@ -1430,34 +1469,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>gpt-4o</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>gpt-4-turbo-2024-04-09</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>mixtral8x7b</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>claude-instant-v1</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>llama3-70b-8192</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>claude-2.1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>gemma-8b-it</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>llama2-70b-chat</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>claude-2</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>gpt-3.5-turbo-0125</c:v>
                 </c:pt>
               </c:strCache>
@@ -1465,35 +1507,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$3:$I$11</c:f>
+              <c:f>Sheet1!$I$3:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>0.64515</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.59695087719298201</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.55130000000000001</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.54669920634920599</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.51661111111111102</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.51415</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.49543134328358196</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.49458478260869548</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.48072962962962951</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.39387391304347796</c:v>
                 </c:pt>
               </c:numCache>
@@ -3305,13 +3350,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3341,13 +3386,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>350045</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>11905</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>33338</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>154780</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3379,14 +3424,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>345279</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>51194</xdr:rowOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>51193</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>23811</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>107155</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3681,10 +3726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O77" sqref="O77"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3695,19 +3740,22 @@
     <col min="6" max="8" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C1" s="6" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="O1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -3735,305 +3783,638 @@
       <c r="I2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.3548</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.34920000000000001</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.94110000000000005</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.94110000000000005</v>
+      </c>
+      <c r="I3" s="6">
+        <f>AVERAGE(H3,E3)</f>
+        <v>0.64515</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C4" s="4">
         <v>0.42253521126760502</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D4" s="4">
         <v>0.25806451612903197</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E4" s="4">
         <v>0.28070175438596401</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F4" s="4">
         <v>0.91420000000000001</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G4" s="4">
         <v>0.91610000000000003</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H4" s="4">
         <v>0.91320000000000001</v>
       </c>
-      <c r="I3" s="7">
-        <f>AVERAGE(H3,E3)</f>
+      <c r="I4" s="6">
+        <f>AVERAGE(H4,E4)</f>
         <v>0.59695087719298201</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="O4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C5" s="4">
         <v>0.49295774647887303</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D5" s="4">
         <v>0.38709677419354799</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E5" s="4">
         <v>0.4</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F5" s="4">
         <v>0.70579999999999998</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G5" s="4">
         <v>0.70879999999999999</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H5" s="4">
         <v>0.7026</v>
       </c>
-      <c r="I4" s="7">
-        <f>AVERAGE(H4,E4)</f>
+      <c r="I5" s="6">
+        <f>AVERAGE(H5,E5)</f>
         <v>0.55130000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="O5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C6" s="4">
         <v>0.47887323943661902</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D6" s="4">
         <v>0.41935483870967699</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E6" s="4">
         <v>0.41269841269841201</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F6" s="4">
         <v>0.68569999999999998</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G6" s="4">
         <v>0.7006</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H6" s="4">
         <v>0.68069999999999997</v>
       </c>
-      <c r="I5" s="7">
-        <f>AVERAGE(H5,E5)</f>
+      <c r="I6" s="6">
+        <f>AVERAGE(H6,E6)</f>
         <v>0.54669920634920599</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="O6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C7" s="4">
         <v>0.50704225352112597</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D7" s="4">
         <v>0.16129032258064499</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E7" s="4">
         <v>0.22222222222222199</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F7" s="4">
         <v>0.81420000000000003</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G7" s="4">
         <v>0.81410000000000005</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H7" s="4">
         <v>0.81100000000000005</v>
       </c>
-      <c r="I6" s="7">
-        <f>AVERAGE(H6,E6)</f>
+      <c r="I7" s="6">
+        <f>AVERAGE(H7,E7)</f>
         <v>0.51661111111111102</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="O7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C8" s="4">
         <v>0.40845070422535201</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D8" s="4">
         <v>0.29032258064516098</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E8" s="4">
         <v>0.3</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F8" s="4">
         <v>0.72719999999999996</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G8" s="4">
         <v>0.73609999999999998</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H8" s="4">
         <v>0.72829999999999995</v>
       </c>
-      <c r="I7" s="7">
-        <f>AVERAGE(H7,E7)</f>
+      <c r="I8" s="6">
+        <f>AVERAGE(H8,E8)</f>
         <v>0.51415</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="O8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C9" s="4">
         <v>0.53521126760563298</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D9" s="4">
         <v>0.54838709677419295</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E9" s="4">
         <v>0.50746268656716398</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F9" s="4">
         <v>0.48570000000000002</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G9" s="4">
         <v>0.49909999999999999</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H9" s="4">
         <v>0.4834</v>
       </c>
-      <c r="I8" s="7">
-        <f>AVERAGE(H8,E8)</f>
+      <c r="I9" s="6">
+        <f>AVERAGE(H9,E9)</f>
         <v>0.49543134328358196</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="O9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C10" s="4">
         <v>0.52112676056338003</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D10" s="4">
         <v>0.19354838709677399</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E10" s="4">
         <v>0.26086956521739102</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F10" s="4">
         <v>0.61529999999999996</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G10" s="4">
         <v>0.73609999999999998</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H10" s="4">
         <v>0.72829999999999995</v>
       </c>
-      <c r="I9" s="7">
-        <f>AVERAGE(H9,E9)</f>
+      <c r="I10" s="6">
+        <f>AVERAGE(H10,E10)</f>
         <v>0.49458478260869548</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="O10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C11" s="4">
         <v>0.43661971830985902</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.225806451612903</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0.25925925925925902</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0.70140000000000002</v>
-      </c>
-      <c r="H10" s="4">
-        <v>0.70220000000000005</v>
-      </c>
-      <c r="I10" s="7">
-        <f>AVERAGE(H10,E10)</f>
-        <v>0.48072962962962951</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0.54929577464788704</v>
       </c>
       <c r="D11" s="4">
         <v>0.225806451612903</v>
       </c>
       <c r="E11" s="4">
+        <v>0.25925925925925902</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.70140000000000002</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0.70220000000000005</v>
+      </c>
+      <c r="I11" s="6">
+        <f>AVERAGE(H11,E11)</f>
+        <v>0.48072962962962951</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.54929577464788704</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.225806451612903</v>
+      </c>
+      <c r="E12" s="4">
         <v>0.30434782608695599</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F12" s="4">
         <v>0.62309999999999999</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G12" s="4">
         <v>0.49909999999999999</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H12" s="4">
         <v>0.4834</v>
       </c>
-      <c r="I11" s="7">
-        <f>AVERAGE(H11,E11)</f>
+      <c r="I12" s="6">
+        <f>AVERAGE(H12,E12)</f>
         <v>0.39387391304347796</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
+      <c r="O16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="O17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O68">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I11">
-    <sortCondition descending="1" ref="I3:I11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I12">
+    <sortCondition descending="1" ref="I3:I12"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="C1:E1"/>

</xml_diff>